<commit_message>
continued work on incomde_benefit API calls good
</commit_message>
<xml_diff>
--- a/2020_income_benefit.xlsx
+++ b/2020_income_benefit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\Desktop\Code_Louisville\DA_2_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\Desktop\Code_Louisville\DA_2_Project\US-county-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72980FBF-18CE-4CF2-A11C-3BB0016F12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3CA320-FD57-49C9-9BB1-482CFBA574FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{601049C5-388A-4C7A-A55E-EEDA92BC393A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{601049C5-388A-4C7A-A55E-EEDA92BC393A}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="314">
   <si>
     <t>not required</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>Number of Rows</t>
-  </si>
-  <si>
     <t>Description:</t>
   </si>
   <si>
@@ -129,15 +126,6 @@
     <t>DP03</t>
   </si>
   <si>
-    <t>DP03_0051PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Total households</t>
-  </si>
-  <si>
-    <t>DP03_0051PEA, DP03_0051PM, DP03_0051PMA</t>
-  </si>
-  <si>
     <t>DP03_0052E</t>
   </si>
   <si>
@@ -366,15 +354,6 @@
     <t>DP03_0064EA, DP03_0064M, DP03_0064MA</t>
   </si>
   <si>
-    <t>DP03_0064PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Total households!!With earnings</t>
-  </si>
-  <si>
-    <t>DP03_0064PEA, DP03_0064PM, DP03_0064PMA</t>
-  </si>
-  <si>
     <t>DP03_0065E</t>
   </si>
   <si>
@@ -564,15 +543,6 @@
     <t>DP03_0075EA, DP03_0075M, DP03_0075MA</t>
   </si>
   <si>
-    <t>DP03_0075PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Families</t>
-  </si>
-  <si>
-    <t>DP03_0075PEA, DP03_0075PM, DP03_0075PMA</t>
-  </si>
-  <si>
     <t>DP03_0076E</t>
   </si>
   <si>
@@ -798,15 +768,6 @@
     <t>DP03_0088EA, DP03_0088M, DP03_0088MA</t>
   </si>
   <si>
-    <t>DP03_0088PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Per capita income (dollars)</t>
-  </si>
-  <si>
-    <t>DP03_0088PEA, DP03_0088PM, DP03_0088PMA</t>
-  </si>
-  <si>
     <t>DP03_0089E</t>
   </si>
   <si>
@@ -816,15 +777,6 @@
     <t>DP03_0089EA, DP03_0089M, DP03_0089MA</t>
   </si>
   <si>
-    <t>DP03_0089PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Nonfamily households</t>
-  </si>
-  <si>
-    <t>DP03_0089PEA, DP03_0089PM, DP03_0089PMA</t>
-  </si>
-  <si>
     <t>DP03_0090E</t>
   </si>
   <si>
@@ -870,15 +822,6 @@
     <t>DP03_0092EA, DP03_0092M, DP03_0092MA</t>
   </si>
   <si>
-    <t>DP03_0092PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Median earnings for workers (dollars)</t>
-  </si>
-  <si>
-    <t>DP03_0092PEA, DP03_0092PM, DP03_0092PMA</t>
-  </si>
-  <si>
     <t>DP03_0093E</t>
   </si>
   <si>
@@ -888,15 +831,6 @@
     <t>DP03_0093EA, DP03_0093M, DP03_0093MA</t>
   </si>
   <si>
-    <t>DP03_0093PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Median earnings for male full-time, year-round workers (dollars)</t>
-  </si>
-  <si>
-    <t>DP03_0093PEA, DP03_0093PM, DP03_0093PMA</t>
-  </si>
-  <si>
     <t>DP03_0094E</t>
   </si>
   <si>
@@ -906,15 +840,6 @@
     <t>DP03_0094EA, DP03_0094M, DP03_0094MA</t>
   </si>
   <si>
-    <t>DP03_0094PE</t>
-  </si>
-  <si>
-    <t>Percent!!INCOME AND BENEFITS (IN 2020 INFLATION-ADJUSTED DOLLARS)!!Median earnings for female full-time, year-round workers (dollars)</t>
-  </si>
-  <si>
-    <t>DP03_0094PEA, DP03_0094PM, DP03_0094PMA</t>
-  </si>
-  <si>
     <t>total_households</t>
   </si>
   <si>
@@ -1002,9 +927,6 @@
     <t>Median earnings for female full-time, year-round workers (dollars)</t>
   </si>
   <si>
-    <t>DP03_0051E,DP03_0051PE</t>
-  </si>
-  <si>
     <t>DF_total_households</t>
   </si>
   <si>
@@ -1014,9 +936,6 @@
     <t>DF_th_range</t>
   </si>
   <si>
-    <t>DP03_0064E,DP03_0064PE</t>
-  </si>
-  <si>
     <t>DF_th_w_earn</t>
   </si>
   <si>
@@ -1050,9 +969,6 @@
     <t>DF_th_w_snap</t>
   </si>
   <si>
-    <t>DP03_0075E,DP03_0075PE</t>
-  </si>
-  <si>
     <t>DF_families</t>
   </si>
   <si>
@@ -1065,31 +981,19 @@
     <t>DF_per_capita</t>
   </si>
   <si>
-    <t>DP03_0088E,DP03_0088PE</t>
-  </si>
-  <si>
     <t>DF_non_family</t>
   </si>
   <si>
-    <t>DP03_0089E,DP03_0089PE</t>
-  </si>
-  <si>
     <t>DF_worker_earn</t>
   </si>
   <si>
-    <t>DP03_0092E,DP03_0092PE</t>
-  </si>
-  <si>
     <t>DF_worker_ft_earn_male</t>
   </si>
   <si>
-    <t>DP03_0093E,DP03_0093PE</t>
-  </si>
-  <si>
     <t>DF_worker_ft_earn_female</t>
   </si>
   <si>
-    <t>DP03_0094E,DP03_0094PE</t>
+    <t>Number of Columns</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1251,6 +1155,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1263,9 +1170,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1281,6 +1185,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1598,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A41A83-E888-4071-9A44-D15A2E247917}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,114 +1513,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="10"/>
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="10"/>
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="D9" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="I9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="I9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1725,316 +1630,354 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="J10" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="D11" s="7">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="I11" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="D12" s="7">
+        <v>24</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="I12" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="D13" s="7">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="D14" s="7">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="D15" s="7">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="I15" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="D16" s="7">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="I16" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="D17" s="7">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="I17" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="D18" s="7">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="I18" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="D19" s="7">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="D20" s="7">
+        <v>24</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="D11" s="12">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="I11" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="D12" s="12">
-        <v>20</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="I12" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="D13" s="12">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="I13" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="D25" s="7">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="D14" s="12">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="I14" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="D15" s="12">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="I15" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="D16" s="12">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="I16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="D17" s="12">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="I17" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="D18" s="12">
-        <v>2</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="I18" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="D19" s="12">
-        <v>2</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="I19" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="D20" s="12">
-        <v>20</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="I20" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="D21" s="12">
-        <v>2</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="I21" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="D22" s="12">
-        <v>2</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="I22" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="D23" s="12">
-        <v>2</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="I23" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="D24" s="12">
-        <v>2</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="I24" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="D25" s="12">
-        <v>2</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="I25" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="I17:N17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="J10:M10"/>
@@ -2051,44 +1994,6 @@
     <mergeCell ref="I14:N14"/>
     <mergeCell ref="I15:N15"/>
     <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I17:N17"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="I12:N12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{1DAA4FBB-A531-48A1-A0D5-BAAED116EA13}"/>
@@ -2119,19 +2024,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2140,33 +2045,33 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2196,19 +2101,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2217,33 +2122,33 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2253,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEB599A-F2FC-475A-8D35-859ECEBEB5AB}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,19 +2178,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2294,33 +2199,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2350,19 +2229,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2371,50 +2250,50 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2423,50 +2302,50 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2475,50 +2354,50 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2527,50 +2406,50 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2579,50 +2458,50 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2631,50 +2510,50 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2683,50 +2562,50 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2735,50 +2614,50 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B16" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -2787,50 +2666,50 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2839,33 +2718,33 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2875,10 +2754,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31F40A-9F6A-4BE1-B38F-6E860A28F333}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2895,19 +2774,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2916,33 +2795,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2952,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE449C4-601F-4CEB-ACB9-768667A2894A}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,19 +2825,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -2993,33 +2846,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3029,10 +2856,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2B8FD-837D-4370-981F-C5A322A4D392}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,19 +2876,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -3070,33 +2897,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3106,10 +2907,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614BE658-B54D-405D-9B04-53137A1DE885}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,19 +2927,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -3147,33 +2948,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3183,10 +2958,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E4149-5E2E-404C-9534-71BA222C30A2}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,19 +2978,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -3224,33 +2999,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3262,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F9F9A-ADF6-41B3-809A-AD6C62009CC5}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H33" activeCellId="14" sqref="H5:I5 H7:I7 H9:I9 H11:I11 H13:I13 H15:I15 H17:I17 H19:I19 H21:I21 H23:I23 H25:I25 H27:I27 H29:I29 H31:I31 H33:I33"/>
+    <sheetView topLeftCell="R8" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3278,7 +3027,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3300,7 +3049,7 @@
     </row>
     <row r="3" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -3313,19 +3062,19 @@
       <c r="I3" s="15"/>
       <c r="J3" s="1"/>
       <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -3335,8 +3084,8 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>19</v>
+      <c r="A5" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -3344,24 +3093,24 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="H5" s="14" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="2"/>
       <c r="K5" s="6" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="M5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>316</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -3372,7 +3121,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -3380,24 +3129,24 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="H7" s="14" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="2"/>
       <c r="K7" s="6" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="M7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -3408,7 +3157,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -3416,24 +3165,24 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="H9" s="14" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="2"/>
       <c r="K9" s="6" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="M9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>320</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3444,7 +3193,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -3452,29 +3201,29 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="H11" s="14" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="2"/>
       <c r="K11" s="6" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="M11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -3482,29 +3231,29 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="14" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="2"/>
       <c r="K13" s="6" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="M13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -3512,29 +3261,29 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="H15" s="14" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="2"/>
       <c r="K15" s="6" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="M15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -3542,29 +3291,29 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="H17" s="14" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="2"/>
       <c r="K17" s="6" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="M17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -3572,29 +3321,29 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="H19" s="14" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="2"/>
       <c r="K19" s="6" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="M19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -3602,29 +3351,29 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="H21" s="14" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="2"/>
       <c r="K21" s="6" t="s">
-        <v>333</v>
+        <v>305</v>
       </c>
       <c r="M21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>332</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -3632,29 +3381,29 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="H23" s="14" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="2"/>
       <c r="K23" s="6" t="s">
-        <v>334</v>
+        <v>306</v>
       </c>
       <c r="M23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>335</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -3662,29 +3411,29 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="H25" s="14" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="2"/>
       <c r="K25" s="6" t="s">
-        <v>336</v>
+        <v>308</v>
       </c>
       <c r="M25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>337</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -3692,29 +3441,29 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="H27" s="14" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="2"/>
       <c r="K27" s="6" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="M27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q27" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>339</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3722,29 +3471,29 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="H29" s="14" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="I29" s="14"/>
       <c r="J29" s="2"/>
       <c r="K29" s="6" t="s">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="M29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>341</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3752,29 +3501,29 @@
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="H31" s="14" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="2"/>
       <c r="K31" s="6" t="s">
-        <v>342</v>
+        <v>311</v>
       </c>
       <c r="M31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>343</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3782,53 +3531,28 @@
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="H33" s="14" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="I33" s="14"/>
       <c r="J33" s="2"/>
       <c r="K33" s="6" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="M33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="Q33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>345</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H23:I23"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="A33:F33"/>
@@ -3837,8 +3561,36 @@
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A23:F23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{5FD494B1-B787-455F-AF52-383FF337592D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3865,19 +3617,19 @@
   <sheetData>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -3886,24 +3638,24 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -3912,24 +3664,24 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -3938,24 +3690,24 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -3964,24 +3716,24 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3990,24 +3742,24 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -4016,24 +3768,24 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -4042,24 +3794,24 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -4068,24 +3820,24 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -4094,24 +3846,24 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -4120,24 +3872,24 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" t="s">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -4146,24 +3898,24 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D42" t="s">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -4172,24 +3924,24 @@
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -4198,24 +3950,24 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -4224,26 +3976,26 @@
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D71" t="s">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -4252,24 +4004,24 @@
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D72" t="s">
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -4278,24 +4030,24 @@
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B73" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D73" t="s">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -4304,24 +4056,24 @@
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B74" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74" t="s">
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -4330,24 +4082,24 @@
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="B79" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D79" t="s">
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -4356,24 +4108,24 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B80" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D80" t="s">
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -4382,24 +4134,24 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="C81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -4408,24 +4160,24 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D82" t="s">
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -4434,7 +4186,7 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4444,10 +4196,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA760ED2-5238-463E-993E-8458CBE07A27}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4464,20 +4216,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1">
         <v>0</v>
       </c>
@@ -4485,33 +4237,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4524,7 +4250,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A20" sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4541,19 +4267,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -4562,50 +4288,50 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4614,50 +4340,50 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -4666,50 +4392,50 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -4718,50 +4444,50 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -4770,50 +4496,50 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -4822,50 +4548,50 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -4874,50 +4600,50 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -4926,50 +4652,50 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -4978,50 +4704,50 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -5030,33 +4756,33 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5066,10 +4792,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43028DC1-CA3E-4D52-A323-92EA10BF0480}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5086,19 +4812,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -5107,33 +4833,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5146,7 +4846,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5163,19 +4863,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -5184,33 +4884,33 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5240,19 +4940,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -5261,33 +4961,33 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5317,19 +5017,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -5338,33 +5038,33 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>